<commit_message>
Work on day 8 part 2
</commit_message>
<xml_diff>
--- a/adventofcode/2024/8/antennae.xlsx
+++ b/adventofcode/2024/8/antennae.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GitHub\johnginnane.github.io\adventofcode\2024\8\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87017434-8B36-4F0E-86C1-3CE63E01B903}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32F7324F-D88F-419C-8E26-6EEF0FE341D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20610" yWindow="3060" windowWidth="13740" windowHeight="14370" xr2:uid="{E3CA9C3A-11FA-4ADE-A751-B5A9F763BA1A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="34800" windowHeight="19080" activeTab="1" xr2:uid="{E3CA9C3A-11FA-4ADE-A751-B5A9F763BA1A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1 (2)" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="55">
   <si>
     <t>A</t>
   </si>
@@ -148,6 +149,57 @@
   </si>
   <si>
     <t>c,e</t>
+  </si>
+  <si>
+    <t>1, 0</t>
+  </si>
+  <si>
+    <t>11, 5</t>
+  </si>
+  <si>
+    <t>5, 7</t>
+  </si>
+  <si>
+    <t>2, 8</t>
+  </si>
+  <si>
+    <t>4, 9</t>
+  </si>
+  <si>
+    <t>1, 10</t>
+  </si>
+  <si>
+    <t>3, 11</t>
+  </si>
+  <si>
+    <t>0, 0</t>
+  </si>
+  <si>
+    <t>1, 1</t>
+  </si>
+  <si>
+    <t>2, 2</t>
+  </si>
+  <si>
+    <t>3, 3</t>
+  </si>
+  <si>
+    <t>4, 4</t>
+  </si>
+  <si>
+    <t>5, 5</t>
+  </si>
+  <si>
+    <t>6, 6</t>
+  </si>
+  <si>
+    <t>8, 8</t>
+  </si>
+  <si>
+    <t>9, 9</t>
+  </si>
+  <si>
+    <t>11, 11</t>
   </si>
 </sst>
 </file>
@@ -178,7 +230,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -230,6 +282,24 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="3"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -347,7 +417,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -395,9 +465,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
@@ -411,6 +478,52 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -858,6 +971,461 @@
         <a:xfrm flipH="1" flipV="1">
           <a:off x="1295400" y="666750"/>
           <a:ext cx="1333500" cy="1752600"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>154781</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="2" name="Straight Connector 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{346A512A-3EEB-4D8B-8007-6AD094E80260}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="381000" y="190500"/>
+          <a:ext cx="1393031" cy="2286000"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>220266</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>184547</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>220266</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>5953</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="3" name="Straight Connector 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2E71485E-7CDF-4C99-B431-A42F611A1B73}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="220266" y="565547"/>
+          <a:ext cx="2714625" cy="773906"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>160734</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>154781</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="4" name="Straight Connector 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7D396542-699F-4064-9BC0-7DB341DA526B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="386953" y="190500"/>
+          <a:ext cx="2553891" cy="1107281"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>5953</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>184547</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>148828</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>148828</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="5" name="Straight Connector 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E22234BE-651C-41E3-91D5-40FCC63F7B1F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="232172" y="184547"/>
+          <a:ext cx="2405062" cy="1488281"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>220266</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>65484</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>220266</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>101203</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="6" name="Straight Connector 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00F5FDC1-100E-4C1A-98F5-033DEB28912C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="220266" y="255984"/>
+          <a:ext cx="2714625" cy="797719"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>41672</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>184547</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>71437</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="7" name="Straight Connector 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AD8481D6-D1C7-44B1-A635-B284ACE72DC0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="946547" y="184547"/>
+          <a:ext cx="1387078" cy="2291953"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>220266</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>5953</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>5953</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="23" name="Straight Connector 22">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7AEEDD90-5731-477B-A599-A7EF592054D0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="220266" y="2857500"/>
+          <a:ext cx="2726531" cy="2291953"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>5953</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>178594</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="34" name="Straight Connector 33">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3320C9CF-5B98-4D51-90F8-DAE76A5675A2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="869156" y="2863453"/>
+          <a:ext cx="1797844" cy="2280047"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>101204</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>178594</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>77391</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>172641</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="38" name="Straight Connector 37">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B842576F-DA80-40E2-8A8F-1BACA8D1754C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="779860" y="2845594"/>
+          <a:ext cx="2012156" cy="2280047"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -1182,7 +1750,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2AA357AB-EB33-4C82-A044-668B6FA58571}">
   <dimension ref="A1:T25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
       <selection activeCell="O13" sqref="O13:P14"/>
     </sheetView>
   </sheetViews>
@@ -1220,7 +1788,7 @@
       <c r="J1" s="8">
         <v>8</v>
       </c>
-      <c r="K1" s="17">
+      <c r="K1" s="8">
         <v>9</v>
       </c>
       <c r="L1" s="8">
@@ -1229,10 +1797,10 @@
       <c r="M1" s="9">
         <v>11</v>
       </c>
-      <c r="O1" s="18" t="s">
+      <c r="O1" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="18" t="s">
+      <c r="P1" s="17" t="s">
         <v>15</v>
       </c>
     </row>
@@ -1242,10 +1810,10 @@
       </c>
       <c r="H2" s="13"/>
       <c r="M2" s="14"/>
-      <c r="O2" s="22" t="s">
+      <c r="O2" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="P2" s="22">
+      <c r="P2" s="21">
         <v>1</v>
       </c>
     </row>
@@ -1258,10 +1826,10 @@
         <v>0</v>
       </c>
       <c r="M3" s="2"/>
-      <c r="O3" s="22" t="s">
+      <c r="O3" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="P3" s="22">
+      <c r="P3" s="21">
         <v>1</v>
       </c>
     </row>
@@ -1275,10 +1843,10 @@
       </c>
       <c r="L4" s="13"/>
       <c r="M4" s="2"/>
-      <c r="O4" s="24" t="s">
+      <c r="O4" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="P4" s="24">
+      <c r="P4" s="23">
         <v>2</v>
       </c>
     </row>
@@ -1291,10 +1859,10 @@
         <v>0</v>
       </c>
       <c r="M5" s="2"/>
-      <c r="O5" s="23" t="s">
+      <c r="O5" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="P5" s="23">
+      <c r="P5" s="22">
         <v>1</v>
       </c>
     </row>
@@ -1307,10 +1875,10 @@
       </c>
       <c r="K6" s="12"/>
       <c r="M6" s="2"/>
-      <c r="O6" s="22" t="s">
+      <c r="O6" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="P6" s="22">
+      <c r="P6" s="21">
         <v>1</v>
       </c>
     </row>
@@ -1319,14 +1887,14 @@
         <v>5</v>
       </c>
       <c r="C7" s="13"/>
-      <c r="H7" s="20" t="s">
+      <c r="H7" s="19" t="s">
         <v>0</v>
       </c>
       <c r="M7" s="2"/>
-      <c r="O7" s="22" t="s">
+      <c r="O7" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="P7" s="22">
+      <c r="P7" s="21">
         <v>1</v>
       </c>
     </row>
@@ -1336,10 +1904,10 @@
       </c>
       <c r="E8" s="13"/>
       <c r="M8" s="2"/>
-      <c r="O8" s="22" t="s">
+      <c r="O8" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="P8" s="22">
+      <c r="P8" s="21">
         <v>1</v>
       </c>
     </row>
@@ -1350,10 +1918,10 @@
       <c r="B9" s="13"/>
       <c r="I9" s="15"/>
       <c r="M9" s="2"/>
-      <c r="O9" s="22" t="s">
+      <c r="O9" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="P9" s="22">
+      <c r="P9" s="21">
         <v>1</v>
       </c>
     </row>
@@ -1365,10 +1933,10 @@
         <v>0</v>
       </c>
       <c r="M10" s="2"/>
-      <c r="O10" s="22" t="s">
+      <c r="O10" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="P10" s="22">
+      <c r="P10" s="21">
         <v>1</v>
       </c>
     </row>
@@ -1380,10 +1948,10 @@
         <v>0</v>
       </c>
       <c r="M11" s="2"/>
-      <c r="O11" s="22" t="s">
+      <c r="O11" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="P11" s="22">
+      <c r="P11" s="21">
         <v>1</v>
       </c>
     </row>
@@ -1393,10 +1961,10 @@
       </c>
       <c r="L12" s="15"/>
       <c r="M12" s="2"/>
-      <c r="O12" s="22" t="s">
+      <c r="O12" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="P12" s="22">
+      <c r="P12" s="21">
         <v>1</v>
       </c>
     </row>
@@ -1416,18 +1984,18 @@
       <c r="K13" s="3"/>
       <c r="L13" s="16"/>
       <c r="M13" s="4"/>
-      <c r="O13" s="23" t="s">
+      <c r="O13" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="P13" s="23">
+      <c r="P13" s="22">
         <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="O14" s="23" t="s">
+      <c r="O14" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="P14" s="23">
+      <c r="P14" s="22">
         <v>1</v>
       </c>
     </row>
@@ -1438,10 +2006,10 @@
       <c r="J15" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="O15" s="23" t="s">
+      <c r="O15" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="P15" s="23">
+      <c r="P15" s="22">
         <v>1</v>
       </c>
     </row>
@@ -1463,11 +2031,11 @@
         <f>"2,1"</f>
         <v>2,1</v>
       </c>
-      <c r="O16" s="19">
+      <c r="O16" s="18">
         <f>COUNTA(O2:O15)</f>
         <v>14</v>
       </c>
-      <c r="P16" s="19">
+      <c r="P16" s="18">
         <f>SUM(P2:P15)</f>
         <v>15</v>
       </c>
@@ -1530,7 +2098,7 @@
         <f>"-2,0"</f>
         <v>-2,0</v>
       </c>
-      <c r="O21" s="21" t="s">
+      <c r="O21" s="20" t="s">
         <v>23</v>
       </c>
       <c r="Q21" t="s">
@@ -1547,7 +2115,7 @@
       </c>
     </row>
     <row r="22" spans="4:20" x14ac:dyDescent="0.25">
-      <c r="O22" s="21" t="s">
+      <c r="O22" s="20" t="s">
         <v>24</v>
       </c>
       <c r="R22" t="s">
@@ -1561,7 +2129,7 @@
       </c>
     </row>
     <row r="23" spans="4:20" x14ac:dyDescent="0.25">
-      <c r="O23" s="21" t="s">
+      <c r="O23" s="20" t="s">
         <v>25</v>
       </c>
       <c r="S23" t="s">
@@ -1572,7 +2140,7 @@
       </c>
     </row>
     <row r="24" spans="4:20" x14ac:dyDescent="0.25">
-      <c r="O24" s="21" t="s">
+      <c r="O24" s="20" t="s">
         <v>26</v>
       </c>
       <c r="T24" t="s">
@@ -1580,8 +2148,832 @@
       </c>
     </row>
     <row r="25" spans="4:20" x14ac:dyDescent="0.25">
-      <c r="O25" s="21" t="s">
+      <c r="O25" s="20" t="s">
         <v>27</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4AF7178-9290-4AC7-82A0-6E9A240D32D4}">
+  <dimension ref="A1:AE36"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="AB10" sqref="AB10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="13" width="3.42578125" style="1" customWidth="1"/>
+    <col min="18" max="30" width="3.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A1" s="7"/>
+      <c r="B1" s="8">
+        <v>0</v>
+      </c>
+      <c r="C1" s="8">
+        <v>1</v>
+      </c>
+      <c r="D1" s="8">
+        <v>2</v>
+      </c>
+      <c r="E1" s="8">
+        <v>3</v>
+      </c>
+      <c r="F1" s="8">
+        <v>4</v>
+      </c>
+      <c r="G1" s="8">
+        <v>5</v>
+      </c>
+      <c r="H1" s="8">
+        <v>6</v>
+      </c>
+      <c r="I1" s="8">
+        <v>7</v>
+      </c>
+      <c r="J1" s="8">
+        <v>8</v>
+      </c>
+      <c r="K1" s="8">
+        <v>9</v>
+      </c>
+      <c r="L1" s="8">
+        <v>10</v>
+      </c>
+      <c r="M1" s="9">
+        <v>11</v>
+      </c>
+      <c r="O1" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="R1" s="7"/>
+      <c r="S1" s="8">
+        <v>0</v>
+      </c>
+      <c r="T1" s="8">
+        <v>1</v>
+      </c>
+      <c r="U1" s="8">
+        <v>2</v>
+      </c>
+      <c r="V1" s="8">
+        <v>3</v>
+      </c>
+      <c r="W1" s="8">
+        <v>4</v>
+      </c>
+      <c r="X1" s="8">
+        <v>5</v>
+      </c>
+      <c r="Y1" s="8">
+        <v>6</v>
+      </c>
+      <c r="Z1" s="8">
+        <v>7</v>
+      </c>
+      <c r="AA1" s="8">
+        <v>8</v>
+      </c>
+      <c r="AB1" s="8">
+        <v>9</v>
+      </c>
+      <c r="AC1" s="8">
+        <v>10</v>
+      </c>
+      <c r="AD1" s="9">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A2" s="5">
+        <v>0</v>
+      </c>
+      <c r="C2" s="13"/>
+      <c r="H2" s="13"/>
+      <c r="M2" s="14"/>
+      <c r="O2" s="28" t="s">
+        <v>38</v>
+      </c>
+      <c r="R2" s="5">
+        <v>0</v>
+      </c>
+      <c r="S2" s="34"/>
+      <c r="T2" s="34"/>
+      <c r="U2" s="24"/>
+      <c r="V2" s="24"/>
+      <c r="W2" s="24"/>
+      <c r="X2" s="24"/>
+      <c r="Y2" s="34"/>
+      <c r="Z2" s="24"/>
+      <c r="AA2" s="24"/>
+      <c r="AB2" s="24"/>
+      <c r="AC2" s="24"/>
+      <c r="AD2" s="37"/>
+      <c r="AE2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A3" s="5">
+        <v>1</v>
+      </c>
+      <c r="E3" s="13"/>
+      <c r="J3" s="10">
+        <v>0</v>
+      </c>
+      <c r="M3" s="2"/>
+      <c r="O3" s="28" t="s">
+        <v>2</v>
+      </c>
+      <c r="R3" s="5">
+        <v>1</v>
+      </c>
+      <c r="S3" s="24"/>
+      <c r="T3" s="34"/>
+      <c r="U3" s="24"/>
+      <c r="V3" s="39"/>
+      <c r="W3" s="24"/>
+      <c r="X3" s="24"/>
+      <c r="Y3" s="24"/>
+      <c r="Z3" s="24"/>
+      <c r="AA3" s="24">
+        <v>0</v>
+      </c>
+      <c r="AB3" s="24"/>
+      <c r="AC3" s="24"/>
+      <c r="AD3" s="26"/>
+      <c r="AE3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A4" s="5">
+        <v>2</v>
+      </c>
+      <c r="F4" s="24"/>
+      <c r="G4" s="10">
+        <v>0</v>
+      </c>
+      <c r="L4" s="13"/>
+      <c r="M4" s="2"/>
+      <c r="O4" s="28" t="s">
+        <v>1</v>
+      </c>
+      <c r="R4" s="5">
+        <v>2</v>
+      </c>
+      <c r="S4" s="24"/>
+      <c r="T4" s="24"/>
+      <c r="U4" s="34"/>
+      <c r="V4" s="24"/>
+      <c r="W4" s="34"/>
+      <c r="X4" s="24">
+        <v>0</v>
+      </c>
+      <c r="Y4" s="24"/>
+      <c r="Z4" s="24"/>
+      <c r="AA4" s="24"/>
+      <c r="AB4" s="24"/>
+      <c r="AC4" s="34"/>
+      <c r="AD4" s="26"/>
+      <c r="AE4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A5" s="5">
+        <v>3</v>
+      </c>
+      <c r="D5" s="13"/>
+      <c r="I5" s="10">
+        <v>0</v>
+      </c>
+      <c r="M5" s="2"/>
+      <c r="O5" s="28" t="s">
+        <v>3</v>
+      </c>
+      <c r="R5" s="5">
+        <v>3</v>
+      </c>
+      <c r="S5" s="24"/>
+      <c r="T5" s="24"/>
+      <c r="U5" s="34"/>
+      <c r="V5" s="34"/>
+      <c r="W5" s="24"/>
+      <c r="X5" s="24"/>
+      <c r="Y5" s="24"/>
+      <c r="Z5" s="24">
+        <v>0</v>
+      </c>
+      <c r="AA5" s="24"/>
+      <c r="AB5" s="24"/>
+      <c r="AC5" s="24"/>
+      <c r="AD5" s="26"/>
+      <c r="AE5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A6" s="5">
+        <v>4</v>
+      </c>
+      <c r="F6" s="10">
+        <v>0</v>
+      </c>
+      <c r="K6" s="12"/>
+      <c r="M6" s="2"/>
+      <c r="O6" s="28" t="s">
+        <v>5</v>
+      </c>
+      <c r="R6" s="5">
+        <v>4</v>
+      </c>
+      <c r="S6" s="24"/>
+      <c r="T6" s="24"/>
+      <c r="U6" s="24"/>
+      <c r="V6" s="24"/>
+      <c r="W6" s="34">
+        <v>0</v>
+      </c>
+      <c r="X6" s="24"/>
+      <c r="Y6" s="24"/>
+      <c r="Z6" s="24"/>
+      <c r="AA6" s="24"/>
+      <c r="AB6" s="38"/>
+      <c r="AC6" s="24"/>
+      <c r="AD6" s="26"/>
+      <c r="AE6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A7" s="5">
+        <v>5</v>
+      </c>
+      <c r="C7" s="13"/>
+      <c r="H7" s="13"/>
+      <c r="M7" s="14"/>
+      <c r="O7" s="28" t="s">
+        <v>6</v>
+      </c>
+      <c r="R7" s="5">
+        <v>5</v>
+      </c>
+      <c r="S7" s="24"/>
+      <c r="T7" s="34"/>
+      <c r="U7" s="24"/>
+      <c r="V7" s="24"/>
+      <c r="W7" s="24"/>
+      <c r="X7" s="34"/>
+      <c r="Y7" s="34" t="s">
+        <v>0</v>
+      </c>
+      <c r="Z7" s="24"/>
+      <c r="AA7" s="24"/>
+      <c r="AB7" s="24"/>
+      <c r="AC7" s="24"/>
+      <c r="AD7" s="37"/>
+      <c r="AE7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A8" s="5">
+        <v>6</v>
+      </c>
+      <c r="E8" s="13"/>
+      <c r="M8" s="2"/>
+      <c r="O8" s="28" t="s">
+        <v>7</v>
+      </c>
+      <c r="R8" s="5">
+        <v>6</v>
+      </c>
+      <c r="S8" s="24"/>
+      <c r="T8" s="24"/>
+      <c r="U8" s="24"/>
+      <c r="V8" s="34"/>
+      <c r="W8" s="24"/>
+      <c r="X8" s="24"/>
+      <c r="Y8" s="34"/>
+      <c r="Z8" s="24"/>
+      <c r="AA8" s="24"/>
+      <c r="AB8" s="24"/>
+      <c r="AC8" s="24"/>
+      <c r="AD8" s="26"/>
+      <c r="AE8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A9" s="5">
+        <v>7</v>
+      </c>
+      <c r="B9" s="13"/>
+      <c r="G9" s="13"/>
+      <c r="I9" s="24"/>
+      <c r="M9" s="2"/>
+      <c r="O9" s="28" t="s">
+        <v>8</v>
+      </c>
+      <c r="R9" s="5">
+        <v>7</v>
+      </c>
+      <c r="S9" s="34"/>
+      <c r="T9" s="24"/>
+      <c r="U9" s="24"/>
+      <c r="V9" s="24"/>
+      <c r="W9" s="24"/>
+      <c r="X9" s="34"/>
+      <c r="Y9" s="24"/>
+      <c r="Z9" s="34"/>
+      <c r="AA9" s="24"/>
+      <c r="AB9" s="24"/>
+      <c r="AC9" s="24"/>
+      <c r="AD9" s="26"/>
+      <c r="AE9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A10" s="5">
+        <v>8</v>
+      </c>
+      <c r="D10" s="13"/>
+      <c r="J10" s="24"/>
+      <c r="M10" s="2"/>
+      <c r="O10" s="28" t="s">
+        <v>16</v>
+      </c>
+      <c r="R10" s="5">
+        <v>8</v>
+      </c>
+      <c r="S10" s="24"/>
+      <c r="T10" s="24"/>
+      <c r="U10" s="34"/>
+      <c r="V10" s="24"/>
+      <c r="W10" s="24"/>
+      <c r="X10" s="24"/>
+      <c r="Y10" s="24"/>
+      <c r="Z10" s="24"/>
+      <c r="AA10" s="34" t="s">
+        <v>0</v>
+      </c>
+      <c r="AB10" s="24"/>
+      <c r="AC10" s="24"/>
+      <c r="AD10" s="26"/>
+      <c r="AE10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A11" s="5">
+        <v>9</v>
+      </c>
+      <c r="F11" s="13"/>
+      <c r="K11" s="24"/>
+      <c r="M11" s="2"/>
+      <c r="O11" s="28" t="s">
+        <v>39</v>
+      </c>
+      <c r="R11" s="5">
+        <v>9</v>
+      </c>
+      <c r="S11" s="24"/>
+      <c r="T11" s="24"/>
+      <c r="U11" s="24"/>
+      <c r="V11" s="24"/>
+      <c r="W11" s="34"/>
+      <c r="X11" s="24"/>
+      <c r="Y11" s="24"/>
+      <c r="Z11" s="24"/>
+      <c r="AA11" s="24"/>
+      <c r="AB11" s="34" t="s">
+        <v>0</v>
+      </c>
+      <c r="AC11" s="24"/>
+      <c r="AD11" s="26"/>
+      <c r="AE11">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A12" s="5">
+        <v>10</v>
+      </c>
+      <c r="C12" s="13"/>
+      <c r="L12" s="24"/>
+      <c r="M12" s="2"/>
+      <c r="O12" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="R12" s="5">
+        <v>10</v>
+      </c>
+      <c r="S12" s="24"/>
+      <c r="T12" s="34"/>
+      <c r="U12" s="24"/>
+      <c r="V12" s="24"/>
+      <c r="W12" s="24"/>
+      <c r="X12" s="24"/>
+      <c r="Y12" s="24"/>
+      <c r="Z12" s="24"/>
+      <c r="AA12" s="24"/>
+      <c r="AB12" s="24"/>
+      <c r="AC12" s="34"/>
+      <c r="AD12" s="26"/>
+      <c r="AE12">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A13" s="6">
+        <v>11</v>
+      </c>
+      <c r="B13" s="3"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="27"/>
+      <c r="F13" s="3"/>
+      <c r="G13" s="3"/>
+      <c r="H13" s="3"/>
+      <c r="I13" s="3"/>
+      <c r="J13" s="3"/>
+      <c r="K13" s="3"/>
+      <c r="L13" s="25"/>
+      <c r="M13" s="4"/>
+      <c r="O13" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="R13" s="6">
+        <v>11</v>
+      </c>
+      <c r="S13" s="25"/>
+      <c r="T13" s="25"/>
+      <c r="U13" s="25"/>
+      <c r="V13" s="36"/>
+      <c r="W13" s="25"/>
+      <c r="X13" s="25"/>
+      <c r="Y13" s="25"/>
+      <c r="Z13" s="25"/>
+      <c r="AA13" s="25"/>
+      <c r="AB13" s="25"/>
+      <c r="AC13" s="36"/>
+      <c r="AD13" s="35"/>
+      <c r="AE13">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="O14" s="28" t="s">
+        <v>40</v>
+      </c>
+      <c r="AE14">
+        <f>SUM(AE2:AE13)</f>
+        <v>29</v>
+      </c>
+    </row>
+    <row r="15" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A15" s="7"/>
+      <c r="B15" s="8">
+        <v>0</v>
+      </c>
+      <c r="C15" s="8">
+        <v>1</v>
+      </c>
+      <c r="D15" s="8">
+        <v>2</v>
+      </c>
+      <c r="E15" s="8">
+        <v>3</v>
+      </c>
+      <c r="F15" s="8">
+        <v>4</v>
+      </c>
+      <c r="G15" s="8">
+        <v>5</v>
+      </c>
+      <c r="H15" s="8">
+        <v>6</v>
+      </c>
+      <c r="I15" s="8">
+        <v>7</v>
+      </c>
+      <c r="J15" s="8">
+        <v>8</v>
+      </c>
+      <c r="K15" s="8">
+        <v>9</v>
+      </c>
+      <c r="L15" s="8">
+        <v>10</v>
+      </c>
+      <c r="M15" s="9">
+        <v>11</v>
+      </c>
+      <c r="O15" s="28" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="16" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A16" s="5">
+        <v>0</v>
+      </c>
+      <c r="B16" s="30"/>
+      <c r="C16" s="24"/>
+      <c r="D16" s="24"/>
+      <c r="E16" s="24"/>
+      <c r="F16" s="24"/>
+      <c r="G16" s="24"/>
+      <c r="H16" s="24"/>
+      <c r="I16" s="24"/>
+      <c r="J16" s="24"/>
+      <c r="K16" s="24"/>
+      <c r="L16" s="24"/>
+      <c r="M16" s="26"/>
+      <c r="O16" s="28" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A17" s="5">
+        <v>1</v>
+      </c>
+      <c r="B17" s="24"/>
+      <c r="C17" s="30"/>
+      <c r="D17" s="24"/>
+      <c r="E17" s="30"/>
+      <c r="F17" s="24"/>
+      <c r="G17" s="24"/>
+      <c r="H17" s="24"/>
+      <c r="I17" s="24"/>
+      <c r="J17" s="24"/>
+      <c r="K17" s="24"/>
+      <c r="L17" s="24"/>
+      <c r="M17" s="26"/>
+      <c r="O17" s="28" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A18" s="5">
+        <v>2</v>
+      </c>
+      <c r="B18" s="24"/>
+      <c r="C18" s="24"/>
+      <c r="D18" s="30"/>
+      <c r="E18" s="24"/>
+      <c r="F18" s="30"/>
+      <c r="G18" s="24"/>
+      <c r="H18" s="24"/>
+      <c r="I18" s="24"/>
+      <c r="J18" s="24"/>
+      <c r="K18" s="24"/>
+      <c r="L18" s="24"/>
+      <c r="M18" s="26"/>
+      <c r="O18" s="28" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A19" s="5">
+        <v>3</v>
+      </c>
+      <c r="B19" s="24"/>
+      <c r="C19" s="24"/>
+      <c r="D19" s="24"/>
+      <c r="E19" s="30"/>
+      <c r="F19" s="24"/>
+      <c r="G19" s="24"/>
+      <c r="H19" s="24"/>
+      <c r="I19" s="24"/>
+      <c r="J19" s="24"/>
+      <c r="K19" s="24"/>
+      <c r="L19" s="24"/>
+      <c r="M19" s="26"/>
+      <c r="O19" s="18">
+        <f>COUNTA(O2:O18)</f>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A20" s="5">
+        <v>4</v>
+      </c>
+      <c r="B20" s="24"/>
+      <c r="C20" s="24"/>
+      <c r="D20" s="24"/>
+      <c r="E20" s="24"/>
+      <c r="F20" s="30"/>
+      <c r="G20" s="24"/>
+      <c r="H20" s="24"/>
+      <c r="I20" s="24"/>
+      <c r="J20" s="24"/>
+      <c r="K20" s="29"/>
+      <c r="L20" s="24"/>
+      <c r="M20" s="26"/>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A21" s="5">
+        <v>5</v>
+      </c>
+      <c r="B21" s="24"/>
+      <c r="C21" s="24"/>
+      <c r="D21" s="24"/>
+      <c r="E21" s="24"/>
+      <c r="F21" s="24"/>
+      <c r="G21" s="30"/>
+      <c r="H21" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="I21" s="24"/>
+      <c r="J21" s="24"/>
+      <c r="K21" s="24"/>
+      <c r="L21" s="24"/>
+      <c r="M21" s="26"/>
+      <c r="O21" s="20" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A22" s="5">
+        <v>6</v>
+      </c>
+      <c r="B22" s="24"/>
+      <c r="C22" s="24"/>
+      <c r="D22" s="24"/>
+      <c r="E22" s="24"/>
+      <c r="F22" s="24"/>
+      <c r="G22" s="24"/>
+      <c r="H22" s="30"/>
+      <c r="I22" s="24"/>
+      <c r="J22" s="24"/>
+      <c r="K22" s="24"/>
+      <c r="L22" s="24"/>
+      <c r="M22" s="26"/>
+      <c r="O22" s="20" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A23" s="5">
+        <v>7</v>
+      </c>
+      <c r="B23" s="24"/>
+      <c r="C23" s="24"/>
+      <c r="D23" s="24"/>
+      <c r="E23" s="24"/>
+      <c r="F23" s="24"/>
+      <c r="G23" s="24"/>
+      <c r="H23" s="24"/>
+      <c r="I23" s="30"/>
+      <c r="J23" s="24"/>
+      <c r="K23" s="24"/>
+      <c r="L23" s="24"/>
+      <c r="M23" s="26"/>
+      <c r="O23" s="20" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A24" s="5">
+        <v>8</v>
+      </c>
+      <c r="B24" s="24"/>
+      <c r="C24" s="24"/>
+      <c r="D24" s="24"/>
+      <c r="E24" s="24"/>
+      <c r="F24" s="24"/>
+      <c r="G24" s="24"/>
+      <c r="H24" s="24"/>
+      <c r="I24" s="24"/>
+      <c r="J24" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="K24" s="24"/>
+      <c r="L24" s="24"/>
+      <c r="M24" s="26"/>
+      <c r="O24" s="20" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A25" s="5">
+        <v>9</v>
+      </c>
+      <c r="B25" s="24"/>
+      <c r="C25" s="24"/>
+      <c r="D25" s="24"/>
+      <c r="E25" s="24"/>
+      <c r="F25" s="24"/>
+      <c r="G25" s="24"/>
+      <c r="H25" s="24"/>
+      <c r="I25" s="24"/>
+      <c r="J25" s="24"/>
+      <c r="K25" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="L25" s="24"/>
+      <c r="M25" s="26"/>
+      <c r="O25" s="20" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A26" s="5">
+        <v>10</v>
+      </c>
+      <c r="B26" s="24"/>
+      <c r="C26" s="24"/>
+      <c r="D26" s="24"/>
+      <c r="E26" s="24"/>
+      <c r="F26" s="24"/>
+      <c r="G26" s="24"/>
+      <c r="H26" s="24"/>
+      <c r="I26" s="24"/>
+      <c r="J26" s="24"/>
+      <c r="K26" s="24"/>
+      <c r="L26" s="30"/>
+      <c r="M26" s="26"/>
+      <c r="O26" s="20" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A27" s="6">
+        <v>11</v>
+      </c>
+      <c r="B27" s="25"/>
+      <c r="C27" s="25"/>
+      <c r="D27" s="25"/>
+      <c r="E27" s="25"/>
+      <c r="F27" s="25"/>
+      <c r="G27" s="25"/>
+      <c r="H27" s="25"/>
+      <c r="I27" s="25"/>
+      <c r="J27" s="25"/>
+      <c r="K27" s="25"/>
+      <c r="L27" s="32"/>
+      <c r="M27" s="31"/>
+      <c r="O27" s="20" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="O28" s="20" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="O29" s="20" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="O30" s="20" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="O31" s="20" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="O32" s="20" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="33" spans="14:15" x14ac:dyDescent="0.25">
+      <c r="O33" s="20" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="34" spans="14:15" x14ac:dyDescent="0.25">
+      <c r="O34" s="20" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="35" spans="14:15" x14ac:dyDescent="0.25">
+      <c r="O35" s="33" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="36" spans="14:15" x14ac:dyDescent="0.25">
+      <c r="N36">
+        <f>SUM(O36+O19)</f>
+        <v>32</v>
+      </c>
+      <c r="O36">
+        <f>COUNTA(O21:O35)</f>
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>